<commit_message>
Muharrem - LeftNav Update
</commit_message>
<xml_diff>
--- a/src/main/resources/XLSFiles/ScenarioStatus.xlsx
+++ b/src/main/resources/XLSFiles/ScenarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="11">
   <si>
     <t>Create Country</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>09.12.22</t>
+  </si>
+  <si>
+    <t>12.12.22</t>
   </si>
 </sst>
 </file>
@@ -86,7 +89,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -692,6 +695,48 @@
         <v>9</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Muharrem - FormContent Update
</commit_message>
<xml_diff>
--- a/src/main/resources/XLSFiles/ScenarioStatus.xlsx
+++ b/src/main/resources/XLSFiles/ScenarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="33">
   <si>
     <t>Create Country</t>
   </si>
@@ -47,43 +47,70 @@
     <t>12.12.22</t>
   </si>
   <si>
-    <t>14.12.22</t>
+    <t>13.12.22</t>
+  </si>
+  <si>
+    <t>Add Document Types</t>
+  </si>
+  <si>
+    <t>16.12.22</t>
+  </si>
+  <si>
+    <t>17.12.22</t>
+  </si>
+  <si>
+    <t>Edit Document Types</t>
   </si>
   <si>
     <t>18.12.22</t>
   </si>
   <si>
-    <t>Add Document Types</t>
-  </si>
-  <si>
-    <t>Create a Discounts</t>
-  </si>
-  <si>
     <t>19.12.22</t>
   </si>
   <si>
-    <t>Create again the same name Discounts</t>
-  </si>
-  <si>
-    <t>Create a Grade Levels</t>
-  </si>
-  <si>
-    <t>Delete a Discounts</t>
-  </si>
-  <si>
-    <t>Edit a Discounts</t>
-  </si>
-  <si>
-    <t>21.12.22</t>
+    <t>Delete Document Types</t>
+  </si>
+  <si>
+    <t>20.12.22</t>
+  </si>
+  <si>
+    <t>Negative Delete Document Types</t>
   </si>
   <si>
     <t>22.12.22</t>
   </si>
   <si>
-    <t>Create again the same name Nationalities</t>
-  </si>
-  <si>
-    <t>Edit a Nationalities</t>
+    <t>17.01.23</t>
+  </si>
+  <si>
+    <t>Create A Citizenship</t>
+  </si>
+  <si>
+    <t>Create An Existant Citizenship</t>
+  </si>
+  <si>
+    <t>Update the Citizenship</t>
+  </si>
+  <si>
+    <t>Delete the Citizenship</t>
+  </si>
+  <si>
+    <t>Search and delete an unavailable Citizenship</t>
+  </si>
+  <si>
+    <t>Create a Attestations</t>
+  </si>
+  <si>
+    <t>Edit a Attestations</t>
+  </si>
+  <si>
+    <t>Delete a Attestations</t>
+  </si>
+  <si>
+    <t>24.01.23</t>
+  </si>
+  <si>
+    <t>Add School Locations</t>
   </si>
 </sst>
 </file>
@@ -128,7 +155,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -781,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -792,7 +819,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
@@ -801,82 +828,82 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
         <v>14</v>
-      </c>
-      <c r="B50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
         <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" t="s">
-        <v>2</v>
-      </c>
-      <c r="D51" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
         <v>14</v>
-      </c>
-      <c r="B52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
         <v>14</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
@@ -885,12 +912,12 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
@@ -899,26 +926,26 @@
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
@@ -927,26 +954,26 @@
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B59" t="s">
         <v>5</v>
@@ -955,40 +982,40 @@
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C61" t="s">
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B62" t="s">
         <v>5</v>
@@ -997,26 +1024,26 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C63" t="s">
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B64" t="s">
         <v>5</v>
@@ -1025,12 +1052,12 @@
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B65" t="s">
         <v>5</v>
@@ -1039,12 +1066,12 @@
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B66" t="s">
         <v>5</v>
@@ -1053,12 +1080,12 @@
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B67" t="s">
         <v>5</v>
@@ -1067,217 +1094,217 @@
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C68" t="s">
         <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B71" t="s">
         <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B72" t="s">
         <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B73" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D73" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B75" t="s">
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B76" t="s">
         <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B81" t="s">
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D81" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B82" t="s">
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83">
@@ -1288,220 +1315,262 @@
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B85" t="s">
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D85" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B87" t="s">
         <v>1</v>
       </c>
       <c r="C87" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B88" t="s">
         <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B89" t="s">
         <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B90" t="s">
         <v>5</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B91" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
+        <v>30</v>
+      </c>
+      <c r="B92" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s">
         <v>22</v>
-      </c>
-      <c r="B92" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" t="s">
-        <v>8</v>
-      </c>
-      <c r="D92" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B93" t="s">
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B94" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B96" t="s">
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D96" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B97" t="s">
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>32</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>32</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>32</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Muharrem - FormContent Update, Add School Locations (#77)
* Muharrem - FormContent Update

* Muharrem - Add School Locations
</commit_message>
<xml_diff>
--- a/src/main/resources/XLSFiles/ScenarioStatus.xlsx
+++ b/src/main/resources/XLSFiles/ScenarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="33">
   <si>
     <t>Create Country</t>
   </si>
@@ -47,43 +47,70 @@
     <t>12.12.22</t>
   </si>
   <si>
-    <t>14.12.22</t>
+    <t>13.12.22</t>
+  </si>
+  <si>
+    <t>Add Document Types</t>
+  </si>
+  <si>
+    <t>16.12.22</t>
+  </si>
+  <si>
+    <t>17.12.22</t>
+  </si>
+  <si>
+    <t>Edit Document Types</t>
   </si>
   <si>
     <t>18.12.22</t>
   </si>
   <si>
-    <t>Add Document Types</t>
-  </si>
-  <si>
-    <t>Create a Discounts</t>
-  </si>
-  <si>
     <t>19.12.22</t>
   </si>
   <si>
-    <t>Create again the same name Discounts</t>
-  </si>
-  <si>
-    <t>Create a Grade Levels</t>
-  </si>
-  <si>
-    <t>Delete a Discounts</t>
-  </si>
-  <si>
-    <t>Edit a Discounts</t>
-  </si>
-  <si>
-    <t>21.12.22</t>
+    <t>Delete Document Types</t>
+  </si>
+  <si>
+    <t>20.12.22</t>
+  </si>
+  <si>
+    <t>Negative Delete Document Types</t>
   </si>
   <si>
     <t>22.12.22</t>
   </si>
   <si>
-    <t>Create again the same name Nationalities</t>
-  </si>
-  <si>
-    <t>Edit a Nationalities</t>
+    <t>17.01.23</t>
+  </si>
+  <si>
+    <t>Create A Citizenship</t>
+  </si>
+  <si>
+    <t>Create An Existant Citizenship</t>
+  </si>
+  <si>
+    <t>Update the Citizenship</t>
+  </si>
+  <si>
+    <t>Delete the Citizenship</t>
+  </si>
+  <si>
+    <t>Search and delete an unavailable Citizenship</t>
+  </si>
+  <si>
+    <t>Create a Attestations</t>
+  </si>
+  <si>
+    <t>Edit a Attestations</t>
+  </si>
+  <si>
+    <t>Delete a Attestations</t>
+  </si>
+  <si>
+    <t>24.01.23</t>
+  </si>
+  <si>
+    <t>Add School Locations</t>
   </si>
 </sst>
 </file>
@@ -128,7 +155,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -781,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -792,7 +819,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B48" t="s">
         <v>1</v>
@@ -801,82 +828,82 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
         <v>14</v>
-      </c>
-      <c r="B50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
         <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" t="s">
-        <v>2</v>
-      </c>
-      <c r="D51" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
         <v>14</v>
-      </c>
-      <c r="B52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
         <v>14</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
@@ -885,12 +912,12 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
@@ -899,26 +926,26 @@
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
@@ -927,26 +954,26 @@
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B59" t="s">
         <v>5</v>
@@ -955,40 +982,40 @@
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C61" t="s">
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B62" t="s">
         <v>5</v>
@@ -997,26 +1024,26 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C63" t="s">
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B64" t="s">
         <v>5</v>
@@ -1025,12 +1052,12 @@
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B65" t="s">
         <v>5</v>
@@ -1039,12 +1066,12 @@
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B66" t="s">
         <v>5</v>
@@ -1053,12 +1080,12 @@
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B67" t="s">
         <v>5</v>
@@ -1067,217 +1094,217 @@
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C68" t="s">
         <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B71" t="s">
         <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B72" t="s">
         <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B73" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D73" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B75" t="s">
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B76" t="s">
         <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B81" t="s">
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D81" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B82" t="s">
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83">
@@ -1288,220 +1315,262 @@
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B85" t="s">
         <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D85" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B87" t="s">
         <v>1</v>
       </c>
       <c r="C87" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D87" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B88" t="s">
         <v>1</v>
       </c>
       <c r="C88" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B89" t="s">
         <v>1</v>
       </c>
       <c r="C89" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B90" t="s">
         <v>5</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B91" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
+        <v>30</v>
+      </c>
+      <c r="B92" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s">
         <v>22</v>
-      </c>
-      <c r="B92" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" t="s">
-        <v>8</v>
-      </c>
-      <c r="D92" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B93" t="s">
         <v>1</v>
       </c>
       <c r="C93" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B94" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B96" t="s">
         <v>1</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D96" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B97" t="s">
         <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>32</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>32</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>32</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>